<commit_message>
De Excel expert heeft het kolommetje breder gemaakt... nu is het weer heel
</commit_message>
<xml_diff>
--- a/Tests/pokkevissen.xlsx
+++ b/Tests/pokkevissen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\AdventOfCode\2021\2021\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198FDA90-7EDA-4801-906F-CCA944B85D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D5BDE7-FCB6-4818-8AA0-CD0F7EC2E597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="610" windowWidth="16770" windowHeight="14360" activeTab="1" xr2:uid="{0D7B6E1E-EF5A-4DF1-95C2-AF4C3CDE9F5B}"/>
+    <workbookView xWindow="550" yWindow="510" windowWidth="24790" windowHeight="14360" activeTab="1" xr2:uid="{0D7B6E1E-EF5A-4DF1-95C2-AF4C3CDE9F5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1556,7 +1556,7 @@
   <cols>
     <col min="2" max="2" width="1.453125" customWidth="1"/>
     <col min="3" max="16" width="4.453125" customWidth="1"/>
-    <col min="259" max="259" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:259" x14ac:dyDescent="0.35">
@@ -2481,7 +2481,7 @@
         <v>234</v>
       </c>
       <c r="ID1">
-        <f t="shared" ref="ID1:JJ1" si="4">IC1+1</f>
+        <f t="shared" ref="ID1:IY1" si="4">IC1+1</f>
         <v>235</v>
       </c>
       <c r="IE1">
@@ -3617,7 +3617,7 @@
         <v>43</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="F4:L4" si="240">C9</f>
+        <f t="shared" ref="H4:L4" si="240">C9</f>
         <v>0</v>
       </c>
       <c r="I4">
@@ -8531,7 +8531,7 @@
         <v>2301875921</v>
       </c>
       <c r="GX8">
-        <f t="shared" ref="GX8:JI8" si="1184">GW9</f>
+        <f t="shared" ref="GX8:IY8" si="1184">GW9</f>
         <v>2080989399</v>
       </c>
       <c r="GY8">
@@ -12690,7 +12690,7 @@
         <v>46446686161</v>
       </c>
       <c r="HK13">
-        <f t="shared" ref="HK13:JJ13" si="1893">SUM(HK3:HK11)</f>
+        <f t="shared" ref="HK13:IY13" si="1893">SUM(HK3:HK11)</f>
         <v>50280015514</v>
       </c>
       <c r="HL13">

</xml_diff>